<commit_message>
fichier excel unique pour les imports
</commit_message>
<xml_diff>
--- a/Imports.xlsx
+++ b/Imports.xlsx
@@ -5,19 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meder\Desktop\BUT\S5\fast-notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nonod\Documents\Etudes\_IUT\3A\FastNotes\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B21DBD-3F70-4ED4-9522-776A6053D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CACEC32-FF6B-4ED0-B031-DC7B97ECDD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="5" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="INFOS-ELEVES" sheetId="1" r:id="rId1"/>
     <sheet name="INFOS-ANNEES" sheetId="2" r:id="rId2"/>
     <sheet name="INFOS-PARCOURS" sheetId="3" r:id="rId3"/>
     <sheet name="INFOS-ENSEIGNEMENTS" sheetId="4" r:id="rId4"/>
-    <sheet name="INFOS-PROFS" sheetId="5" r:id="rId5"/>
+    <sheet name="INFOS-SEMESTRES" sheetId="6" r:id="rId5"/>
+    <sheet name="INFOS-EVALUATIONS" sheetId="10" r:id="rId6"/>
+    <sheet name="INFOS-RESSOURCES" sheetId="7" r:id="rId7"/>
+    <sheet name="INFOS-GROUPES" sheetId="8" r:id="rId8"/>
+    <sheet name="INFOS-UE" sheetId="9" r:id="rId9"/>
+    <sheet name="INFOS-PROFS" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Code</t>
   </si>
@@ -148,13 +153,97 @@
   </si>
   <si>
     <t>prenom</t>
+  </si>
+  <si>
+    <t>libelle</t>
+  </si>
+  <si>
+    <t>annee</t>
+  </si>
+  <si>
+    <t>TEST_5</t>
+  </si>
+  <si>
+    <t>2026-2027</t>
+  </si>
+  <si>
+    <t>TEST_6</t>
+  </si>
+  <si>
+    <t>R5.A04 - Qualité algorithmique</t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>parcours</t>
+  </si>
+  <si>
+    <t>TEST_B</t>
+  </si>
+  <si>
+    <t>tB</t>
+  </si>
+  <si>
+    <t>AGED</t>
+  </si>
+  <si>
+    <t>tC</t>
+  </si>
+  <si>
+    <t>code_competence</t>
+  </si>
+  <si>
+    <t>test 2 import</t>
+  </si>
+  <si>
+    <t>B3FTA4AB</t>
+  </si>
+  <si>
+    <t>test 3 import</t>
+  </si>
+  <si>
+    <t>coefficient</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>date_epreuve</t>
+  </si>
+  <si>
+    <t>date_rattrapage</t>
+  </si>
+  <si>
+    <t>TEST insert 4</t>
+  </si>
+  <si>
+    <t>Ecrit</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:00</t>
+  </si>
+  <si>
+    <t>BFTA5R10</t>
+  </si>
+  <si>
+    <t>TEST insert 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +273,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,10 +307,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -229,9 +333,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +373,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +479,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,17 +631,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761DC1A1-87CF-4EEC-8630-3B548B9394FE}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -577,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -608,6 +712,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D895BB63-EBE1-4430-9E6E-68E9CFB83735}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{3D00F156-F762-4FCF-9DA5-4ADD9F99B977}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{FA880615-95DE-4B2D-B6C2-4BFCE5F1E253}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B074E5-33DB-43A1-8AC1-C29F5F438D54}">
   <dimension ref="A1:B2"/>
@@ -616,12 +794,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -629,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2026</v>
       </c>
@@ -650,12 +828,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -663,7 +841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -684,12 +862,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -700,7 +878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -717,75 +895,259 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D895BB63-EBE1-4430-9E6E-68E9CFB83735}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA881635-AA22-498E-BB63-9C1A5F0CF245}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2454D53-76DA-4241-B881-27A410BE07B2}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC437EF2-9E80-418D-8C1C-E39FEE716E73}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DAAB34-97BD-4552-83E3-17F3E039FBDE}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{3D00F156-F762-4FCF-9DA5-4ADD9F99B977}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{FA880615-95DE-4B2D-B6C2-4BFCE5F1E253}"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EDC0F2-4617-44FC-AB9B-43245FD96FBA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout groupes dans fichier d'imports
</commit_message>
<xml_diff>
--- a/Imports.xlsx
+++ b/Imports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meder\Desktop\BUT\S5\fast-notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leymat Nicolas\Documents\GitLabCours\ProjetTuteuré\New folder\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B21DBD-3F70-4ED4-9522-776A6053D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FD0AC2-BE8E-4DC8-81F6-EFCBD0F12046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
+    <workbookView xWindow="11808" yWindow="2652" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="5" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="INFOS-ELEVES" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="INFOS-PARCOURS" sheetId="3" r:id="rId3"/>
     <sheet name="INFOS-ENSEIGNEMENTS" sheetId="4" r:id="rId4"/>
     <sheet name="INFOS-PROFS" sheetId="5" r:id="rId5"/>
+    <sheet name="INFOS-GROUPES" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Code</t>
   </si>
@@ -148,6 +149,30 @@
   </si>
   <si>
     <t>prenom</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>libelle</t>
+  </si>
+  <si>
+    <t>parcours</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>RAPP_6</t>
+  </si>
+  <si>
+    <t>in_s5_A_2026_2027</t>
+  </si>
+  <si>
+    <t>TestImportsMultiples</t>
+  </si>
+  <si>
+    <t>DACS</t>
   </si>
 </sst>
 </file>
@@ -212,7 +237,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -229,9 +254,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +294,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +400,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,17 +552,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761DC1A1-87CF-4EEC-8630-3B548B9394FE}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -577,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -616,12 +641,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -629,7 +654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2026</v>
       </c>
@@ -650,12 +675,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -663,7 +688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -684,12 +709,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -700,7 +725,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -724,13 +749,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -764,7 +789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -788,4 +813,56 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8916B59-0175-4701-97ED-3DEAF57E7BA5}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix fautes et footer
</commit_message>
<xml_diff>
--- a/Imports.xlsx
+++ b/Imports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nonod\Documents\Etudes\_IUT\3A\FastNotes\fast-notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Informatique\PHP\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4DF481-F3CE-4091-A43F-71A6556CFBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798FBCAD-1476-41EB-A7C5-E080AABF9558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="4" activeTab="7" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="9" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="INFOS-ELEVES" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="INFOS-EPREUVES" sheetId="10" r:id="rId6"/>
     <sheet name="INFOS-RESSOURCES" sheetId="7" r:id="rId7"/>
     <sheet name="INFOS-UE" sheetId="9" r:id="rId8"/>
-    <sheet name="INFOS-PROFS" sheetId="5" r:id="rId9"/>
+    <sheet name="INFOS-GROUPES" sheetId="11" r:id="rId9"/>
+    <sheet name="INFOS-PROFS" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="122">
   <si>
     <t>Code</t>
   </si>
@@ -106,9 +107,6 @@
     <t>BFTA5R01</t>
   </si>
   <si>
-    <t>ProfDeFou</t>
-  </si>
-  <si>
     <t>prof@defou.com</t>
   </si>
   <si>
@@ -118,18 +116,6 @@
     <t>DeFou</t>
   </si>
   <si>
-    <t>ProfDeFou1</t>
-  </si>
-  <si>
-    <t>prof1@defou.com</t>
-  </si>
-  <si>
-    <t>DeFou1</t>
-  </si>
-  <si>
-    <t>Professeur1</t>
-  </si>
-  <si>
     <t>dmm3793a</t>
   </si>
   <si>
@@ -160,24 +146,12 @@
     <t>annee</t>
   </si>
   <si>
-    <t>TEST_5</t>
-  </si>
-  <si>
     <t>2026-2027</t>
   </si>
   <si>
-    <t>TEST_6</t>
-  </si>
-  <si>
     <t>R5.A04 - Qualité algorithmique</t>
   </si>
   <si>
-    <t>TEST3</t>
-  </si>
-  <si>
-    <t>TEST2</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -190,9 +164,6 @@
     <t>B3FTA4AB</t>
   </si>
   <si>
-    <t>test 3 import</t>
-  </si>
-  <si>
     <t>coefficient</t>
   </si>
   <si>
@@ -205,9 +176,6 @@
     <t>date_rattrapage</t>
   </si>
   <si>
-    <t>TEST insert 4</t>
-  </si>
-  <si>
     <t>Ecrit</t>
   </si>
   <si>
@@ -217,7 +185,232 @@
     <t>BFTA5R10</t>
   </si>
   <si>
-    <t>TEST insert 5</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>LIBELLE</t>
+  </si>
+  <si>
+    <t>PARCOURS</t>
+  </si>
+  <si>
+    <t>Test Imports1</t>
+  </si>
+  <si>
+    <t>Test Imports2</t>
+  </si>
+  <si>
+    <t>Test Imports3</t>
+  </si>
+  <si>
+    <t>Test Imports4</t>
+  </si>
+  <si>
+    <t>Test Imports5</t>
+  </si>
+  <si>
+    <t>Test Imports6</t>
+  </si>
+  <si>
+    <t>Test Imports7</t>
+  </si>
+  <si>
+    <t>Test Imports8</t>
+  </si>
+  <si>
+    <t>Test Imports9</t>
+  </si>
+  <si>
+    <t>Test Imports10</t>
+  </si>
+  <si>
+    <t>Test Imports11</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio1</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio2</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio3</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio4</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio5</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio6</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio7</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio8</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio9</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio10</t>
+  </si>
+  <si>
+    <t>in_S5_W_Ratio11</t>
+  </si>
+  <si>
+    <t>AGED</t>
+  </si>
+  <si>
+    <t>RAPP</t>
+  </si>
+  <si>
+    <t>TEST4</t>
+  </si>
+  <si>
+    <t>TEST5</t>
+  </si>
+  <si>
+    <t>TEST6</t>
+  </si>
+  <si>
+    <t>TEST7</t>
+  </si>
+  <si>
+    <t>TEST8</t>
+  </si>
+  <si>
+    <t>TEST9</t>
+  </si>
+  <si>
+    <t>TEST10</t>
+  </si>
+  <si>
+    <t>TEST22</t>
+  </si>
+  <si>
+    <t>TEST33</t>
+  </si>
+  <si>
+    <t>TEST_8</t>
+  </si>
+  <si>
+    <t>TEST_9</t>
+  </si>
+  <si>
+    <t>TEST_10</t>
+  </si>
+  <si>
+    <t>TEST_11</t>
+  </si>
+  <si>
+    <t>TEST_12</t>
+  </si>
+  <si>
+    <t>TEST_13</t>
+  </si>
+  <si>
+    <t>2026-2028</t>
+  </si>
+  <si>
+    <t>2026-2029</t>
+  </si>
+  <si>
+    <t>2026-2030</t>
+  </si>
+  <si>
+    <t>2026-2031</t>
+  </si>
+  <si>
+    <t>2026-2032</t>
+  </si>
+  <si>
+    <t>TEST insert 6</t>
+  </si>
+  <si>
+    <t>TEST insert 7</t>
+  </si>
+  <si>
+    <t>TEST insert 8</t>
+  </si>
+  <si>
+    <t>TEST insert 9</t>
+  </si>
+  <si>
+    <t>TEST insert 10</t>
+  </si>
+  <si>
+    <t>TEST insert 11</t>
+  </si>
+  <si>
+    <t>TEST insert 12</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:01</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:02</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:03</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:04</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:05</t>
+  </si>
+  <si>
+    <t>2024-01-12  00:00:06</t>
+  </si>
+  <si>
+    <t>BFTA5R11</t>
+  </si>
+  <si>
+    <t>BFTA5R12</t>
+  </si>
+  <si>
+    <t>BFTA5R13</t>
+  </si>
+  <si>
+    <t>BFTA5R14</t>
+  </si>
+  <si>
+    <t>BFTA5R15</t>
+  </si>
+  <si>
+    <t>BFTA5R16</t>
+  </si>
+  <si>
+    <t>TEST23</t>
+  </si>
+  <si>
+    <t>TEST24</t>
+  </si>
+  <si>
+    <t>TEST25</t>
+  </si>
+  <si>
+    <t>TEST26</t>
+  </si>
+  <si>
+    <t>TEST27</t>
+  </si>
+  <si>
+    <t>ProfDeFou2</t>
+  </si>
+  <si>
+    <t>ProfDeFou3</t>
+  </si>
+  <si>
+    <t>ProfDeFou4</t>
+  </si>
+  <si>
+    <t>ProfDeFou5</t>
+  </si>
+  <si>
+    <t>ProfDeFou6</t>
   </si>
 </sst>
 </file>
@@ -314,9 +507,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,7 +547,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -460,7 +653,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,7 +795,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -644,19 +837,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>21908212</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -664,19 +857,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>22165854</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -690,6 +883,132 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D895BB63-EBE1-4430-9E6E-68E9CFB83735}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{3D00F156-F762-4FCF-9DA5-4ADD9F99B977}"/>
+    <hyperlink ref="C3:C6" r:id="rId2" display="prof@defou.com" xr:uid="{A1F44BB5-D8E6-4267-81B1-C316C7026B41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -803,68 +1122,101 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA881635-AA22-498E-BB63-9C1A5F0CF245}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2454D53-76DA-4241-B881-27A410BE07B2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
@@ -872,107 +1224,265 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC437EF2-9E80-418D-8C1C-E39FEE716E73}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EDC0F2-4617-44FC-AB9B-43245FD96FBA}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -980,13 +1490,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D2" s="4">
         <v>5</v>
@@ -994,93 +1504,228 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4">
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D895BB63-EBE1-4430-9E6E-68E9CFB83735}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F51DC-2E56-4E79-8156-8134CFC9BC2D}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{3D00F156-F762-4FCF-9DA5-4ADD9F99B977}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{FA880615-95DE-4B2D-B6C2-4BFCE5F1E253}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>